<commit_message>
updated for item count
</commit_message>
<xml_diff>
--- a/nutrition_info.xlsx
+++ b/nutrition_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\OperationsResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A5AB23-63D9-4C3A-B34A-0C12B488A241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0FDEFF-716A-4A5C-9471-FCE79F1FF188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{69B92017-27F2-48BC-A2D7-FB496965E7C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Calories</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Crispy Tender Sandwich</t>
+  </si>
+  <si>
+    <t>Item Count</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B097BC2B-1C8D-4AAC-A42A-58B109DCBDC8}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -473,7 +476,7 @@
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -510,8 +513,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -548,8 +554,11 @@
       <c r="L2" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -586,8 +595,11 @@
       <c r="L3" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="39" x14ac:dyDescent="0.45">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -624,8 +636,11 @@
       <c r="L4" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="39" x14ac:dyDescent="0.45">
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -662,8 +677,11 @@
       <c r="L5" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="39" x14ac:dyDescent="0.45">
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -700,8 +718,11 @@
       <c r="L6" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -738,8 +759,11 @@
       <c r="L7" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="39" x14ac:dyDescent="0.45">
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -776,8 +800,11 @@
       <c r="L8" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -814,8 +841,11 @@
       <c r="L9" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -852,8 +882,11 @@
       <c r="L10" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="39" x14ac:dyDescent="0.45">
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -890,6 +923,191 @@
       <c r="L11" s="1">
         <v>19</v>
       </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>